<commit_message>
Crop suggestion and Translation
</commit_message>
<xml_diff>
--- a/app/src/main/python/soildata.xlsx
+++ b/app/src/main/python/soildata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raju\Android\BetaChatSystem\app\src\main\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C691BE5B-1EF5-480D-9978-35675383134F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C6B9A0-45FD-4FD3-A783-389EFECA983C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCB5DC59-9019-47C5-8D18-1A06D53B827B}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t xml:space="preserve"> deep black</t>
   </si>
   <si>
-    <t>sugercane</t>
-  </si>
-  <si>
     <t>rice</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>July-October</t>
+  </si>
+  <si>
+    <t>sugarcane</t>
   </si>
 </sst>
 </file>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D74EE44-1EE4-4B53-9EA4-174A4CFA194D}">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,7 +1033,7 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -1053,7 +1053,7 @@
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1227,19 +1227,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>43</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>44</v>
-      </c>
-      <c r="E32" t="s">
-        <v>45</v>
       </c>
       <c r="F32" s="3">
         <v>4</v>
@@ -1247,19 +1247,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
         <v>41</v>
       </c>
-      <c r="B33" t="s">
-        <v>42</v>
-      </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
         <v>44</v>
-      </c>
-      <c r="E33" t="s">
-        <v>45</v>
       </c>
       <c r="F33" s="3">
         <v>4</v>
@@ -1267,19 +1267,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
         <v>41</v>
       </c>
-      <c r="B34" t="s">
-        <v>42</v>
-      </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
         <v>44</v>
-      </c>
-      <c r="E34" t="s">
-        <v>45</v>
       </c>
       <c r="F34" s="3">
         <v>4</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
         <v>14</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>14</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
@@ -1447,13 +1447,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
-        <v>50</v>
-      </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
         <v>25</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -1547,10 +1547,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
         <v>52</v>
-      </c>
-      <c r="B48" t="s">
-        <v>53</v>
       </c>
       <c r="C48" t="s">
         <v>12</v>
@@ -1567,13 +1567,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
         <v>52</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>53</v>
-      </c>
-      <c r="C49" t="s">
-        <v>54</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
@@ -1587,13 +1587,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="B50" t="s">
-        <v>53</v>
-      </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -1607,19 +1607,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
         <v>52</v>
-      </c>
-      <c r="B51" t="s">
-        <v>53</v>
       </c>
       <c r="C51" t="s">
         <v>29</v>
       </c>
       <c r="D51" t="s">
+        <v>55</v>
+      </c>
+      <c r="E51" t="s">
         <v>56</v>
-      </c>
-      <c r="E51" t="s">
-        <v>57</v>
       </c>
       <c r="F51" s="3">
         <v>5</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
         <v>32</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>32</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>32</v>
@@ -1767,13 +1767,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
         <v>25</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>38</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>38</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
         <v>38</v>
@@ -1847,13 +1847,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
         <v>38</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D63" t="s">
         <v>25</v>
@@ -1867,13 +1867,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" t="s">
         <v>38</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D64" t="s">
         <v>25</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B65" t="s">
         <v>14</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
         <v>14</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
         <v>14</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
         <v>14</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B69" t="s">
         <v>14</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
         <v>38</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B71" t="s">
         <v>38</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
         <v>38</v>
@@ -2047,13 +2047,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B73" t="s">
         <v>38</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D73" t="s">
         <v>25</v>
@@ -2067,13 +2067,13 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
         <v>38</v>
       </c>
       <c r="C74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D74" t="s">
         <v>25</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
@@ -2167,10 +2167,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79" t="s">
         <v>63</v>
-      </c>
-      <c r="B79" t="s">
-        <v>64</v>
       </c>
       <c r="C79" t="s">
         <v>13</v>
@@ -2187,10 +2187,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" t="s">
         <v>63</v>
-      </c>
-      <c r="B80" t="s">
-        <v>64</v>
       </c>
       <c r="C80" t="s">
         <v>12</v>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" t="s">
         <v>63</v>
-      </c>
-      <c r="B81" t="s">
-        <v>64</v>
       </c>
       <c r="C81" t="s">
         <v>15</v>
@@ -2227,13 +2227,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82" t="s">
         <v>63</v>
       </c>
-      <c r="B82" t="s">
-        <v>64</v>
-      </c>
       <c r="C82" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D82" t="s">
         <v>25</v>
@@ -2247,16 +2247,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>62</v>
+      </c>
+      <c r="B83" t="s">
         <v>63</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" t="s">
         <v>64</v>
-      </c>
-      <c r="C83" t="s">
-        <v>40</v>
-      </c>
-      <c r="D83" t="s">
-        <v>65</v>
       </c>
       <c r="E83" t="s">
         <v>21</v>

</xml_diff>